<commit_message>
fixed IE page, added activity area analys
</commit_message>
<xml_diff>
--- a/meta/Словарь перевода показателей портрета.xlsx
+++ b/meta/Словарь перевода показателей портрета.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaspa_ay\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaspa_ay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
   <si>
     <t>ACTIVE</t>
   </si>
@@ -666,6 +666,12 @@
   </si>
   <si>
     <t>Доля клиентов с флагом, показывающим платит ли клиент заработную плату</t>
+  </si>
+  <si>
+    <t>SP_BIG_PLANS</t>
+  </si>
+  <si>
+    <t>Доля клиентов с ПУ Большие планы</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B107"/>
+  <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,713 +1215,721 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>115</v>
+        <v>214</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>191</v>
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>134</v>
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>192</v>
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>137</v>
+        <v>42</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>197</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>197</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>207</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>210</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>151</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B83" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B86" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>201</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new fields to analys
</commit_message>
<xml_diff>
--- a/meta/Словарь перевода показателей портрета.xlsx
+++ b/meta/Словарь перевода показателей портрета.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
   <si>
     <t>ACTIVE</t>
   </si>
@@ -672,6 +672,30 @@
   </si>
   <si>
     <t>Доля клиентов с ПУ Большие планы</t>
+  </si>
+  <si>
+    <t>CASH_INKASS</t>
+  </si>
+  <si>
+    <t>Сумма инкассации</t>
+  </si>
+  <si>
+    <t>CARD_PURCHASES</t>
+  </si>
+  <si>
+    <t>Сумма покупок по карте</t>
+  </si>
+  <si>
+    <t>WALLET_POTENTIAL</t>
+  </si>
+  <si>
+    <t>Средний потенциал кошелька</t>
+  </si>
+  <si>
+    <t>ESCAPE_RKO</t>
+  </si>
+  <si>
+    <t>Доля закрывших РКО</t>
   </si>
 </sst>
 </file>
@@ -750,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -776,6 +800,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1056,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,6 +1958,38 @@
         <v>204</v>
       </c>
     </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" t="s">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>